<commit_message>
Priorization started, few resumes added
</commit_message>
<xml_diff>
--- a/Estado del arte.xlsx
+++ b/Estado del arte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camilo Ortiz\Documents\Universidad de Los Andes\Maestría\Tercer Semestre\Tesis 1\estadodelarte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDE1F2D-B743-46FF-B173-CD76610E7E00}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB367EC-9010-43C4-8645-990B1C9F5ED2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7932" yWindow="4320" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="259">
   <si>
     <t>Titulo del artículo</t>
   </si>
@@ -861,6 +861,15 @@
   </si>
   <si>
     <t>Mobile Crowdsourcing (MCS) is an effective and novel method of data collection and processing. Current MCS generally adopts a centralized architecture by depending on an assumed trusted party. This design easily suffers from single-point failure and cannot be realized in practice since a trusted service provider does not really exist. More dangerously, the centralized party may perform dishonestly and thus harms the benefit and privacy of MCS users. To tackle these problems, we propose a novel blockchain-based MCS system, named MCS-Chain, to realize fully distributed and decentralized trust management in MCS. Aiming at improving the poor efficiency of traditional blockchain technology, we propose a novel consensus mechanism for block generation, which greatly reduces computational overhead. The proposed MCS-Chain system also solves the fork issue and centralization problem suffered by most existing blockchain-based systems. Serious security analysis and experimental evaluation further illustrate the security and efficiency of our system.</t>
+  </si>
+  <si>
+    <t>Prioridad</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Alta</t>
   </si>
 </sst>
 </file>
@@ -1194,10 +1203,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:I55"/>
+  <dimension ref="B2:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1220,7 @@
     <col min="8" max="8" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1236,8 +1245,11 @@
       <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" ht="132" x14ac:dyDescent="0.25">
+      <c r="J2" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="132" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1262,8 +1274,11 @@
       <c r="I3" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="J3" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="79.2" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1288,8 +1303,11 @@
       <c r="I4" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="J4" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="105.6" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1314,8 +1332,11 @@
       <c r="I5" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="J5" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="105.6" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1340,8 +1361,11 @@
       <c r="I6" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.25">
+      <c r="J6" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
@@ -1367,7 +1391,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="66" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="66" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>40</v>
       </c>
@@ -1393,7 +1417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="92.4" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>46</v>
       </c>
@@ -1419,7 +1443,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="224.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="224.4" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>49</v>
       </c>
@@ -1442,7 +1466,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>54</v>
       </c>
@@ -1466,7 +1490,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="105.6" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>58</v>
       </c>
@@ -1492,7 +1516,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>64</v>
       </c>
@@ -1518,7 +1542,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="118.8" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
         <v>70</v>
       </c>
@@ -1544,7 +1568,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="92.4" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
         <v>75</v>
       </c>
@@ -1570,7 +1594,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="79.2" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>81</v>
       </c>

</xml_diff>